<commit_message>
Split out primary types
</commit_message>
<xml_diff>
--- a/posts/mapoli-primaries-2024/2024 Candidates 6.4.24.xlsx
+++ b/posts/mapoli-primaries-2024/2024 Candidates 6.4.24.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domalley\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbenson/Documents/Repos/ma-primary-races/bwb-blog/posts/mapoli-primaries-2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F63511-310B-7641-9582-630377516B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="District &amp; County Candidates" sheetId="1" r:id="rId1"/>
@@ -3608,7 +3609,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3666,12 +3667,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -3952,25 +3952,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H414"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B396" sqref="B396"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14:G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
     <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="70.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>643</v>
       </c>
@@ -3996,437 +3996,437 @@
         <v>649</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1152</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>1151</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>1147</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>1153</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
         <v>1154</v>
       </c>
-      <c r="H2" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="H2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1152</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>1151</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>1148</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>1155</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="G3"/>
+      <c r="H3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>1152</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>1151</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>1150</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" t="s">
         <v>1156</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" t="s">
         <v>1157</v>
       </c>
-      <c r="H4" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>1152</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>1151</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>1149</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" t="s">
         <v>1158</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" t="s">
         <v>1159</v>
       </c>
-      <c r="H5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>1173</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>600</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>1160</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" t="s">
         <v>1176</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" t="s">
         <v>1057</v>
       </c>
-      <c r="H6" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="H6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>1173</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>601</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>1161</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" t="s">
         <v>1177</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" t="s">
         <v>1057</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>1173</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>602</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>1162</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" t="s">
         <v>1178</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4">
+      <c r="G8"/>
+      <c r="H8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>1173</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>603</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>1163</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" t="s">
         <v>1179</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" t="s">
         <v>1180</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>1173</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>604</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>1164</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" t="s">
         <v>1181</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" t="s">
         <v>1057</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>1173</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>605</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>1165</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" t="s">
         <v>1182</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" t="s">
         <v>1180</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>1173</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>1174</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>1166</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" t="s">
         <v>1183</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" t="s">
         <v>1184</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>1173</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>607</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>1167</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" t="s">
         <v>1185</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" t="s">
         <v>1057</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>1173</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>607</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>1168</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" t="s">
         <v>1186</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4">
+      <c r="G14"/>
+      <c r="H14">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>1173</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>607</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>1169</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" t="s">
         <v>1187</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4">
+      <c r="G15"/>
+      <c r="H15">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>1173</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>607</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>1170</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" t="s">
         <v>1188</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4">
+      <c r="G16"/>
+      <c r="H16">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>1173</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>1175</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>1171</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" t="s">
         <v>1189</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" t="s">
         <v>1190</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:8" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>1173</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>1175</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>1172</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" t="s">
         <v>1191</v>
       </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4">
+      <c r="G18"/>
+      <c r="H18">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>5</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>5</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4700,7 +4700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -4824,7 +4824,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -4876,7 +4876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>26</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>26</v>
       </c>
@@ -4954,7 +4954,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>26</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>26</v>
       </c>
@@ -5006,7 +5006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>26</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -5058,7 +5058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>26</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>26</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>26</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>26</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>26</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>26</v>
       </c>
@@ -5283,7 +5283,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>26</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>26</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>26</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>26</v>
       </c>
@@ -5482,7 +5482,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>26</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>26</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -5580,7 +5580,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -5658,7 +5658,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -5759,7 +5759,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>26</v>
       </c>
@@ -5785,7 +5785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>26</v>
       </c>
@@ -5811,7 +5811,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>26</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -5860,7 +5860,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>26</v>
       </c>
@@ -5886,7 +5886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>26</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>26</v>
       </c>
@@ -5964,7 +5964,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>26</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>26</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>26</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>26</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>26</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>26</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>26</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>26</v>
       </c>
@@ -6267,7 +6267,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>26</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>26</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>26</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>126</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>126</v>
       </c>
@@ -6440,7 +6440,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>126</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>126</v>
       </c>
@@ -6486,7 +6486,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>126</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>126</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>126</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>126</v>
       </c>
@@ -6581,7 +6581,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>126</v>
       </c>
@@ -6604,7 +6604,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>126</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>126</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>126</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>126</v>
       </c>
@@ -6708,7 +6708,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>126</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>126</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>126</v>
       </c>
@@ -6809,7 +6809,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>126</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>126</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>126</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>126</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>126</v>
       </c>
@@ -6936,7 +6936,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>126</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>126</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>126</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>126</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>126</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>126</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -7167,7 +7167,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -7193,7 +7193,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>126</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>126</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>126</v>
       </c>
@@ -7320,7 +7320,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>126</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>126</v>
       </c>
@@ -7372,7 +7372,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>126</v>
       </c>
@@ -7398,7 +7398,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>126</v>
       </c>
@@ -7424,7 +7424,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>126</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>126</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>126</v>
       </c>
@@ -7499,7 +7499,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>126</v>
       </c>
@@ -7522,7 +7522,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>126</v>
       </c>
@@ -7548,7 +7548,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>126</v>
       </c>
@@ -7574,7 +7574,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>126</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>126</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>126</v>
       </c>
@@ -7652,7 +7652,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>126</v>
       </c>
@@ -7675,7 +7675,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>126</v>
       </c>
@@ -7701,7 +7701,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>126</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>126</v>
       </c>
@@ -7753,7 +7753,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>126</v>
       </c>
@@ -7776,7 +7776,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>126</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>126</v>
       </c>
@@ -7828,7 +7828,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>126</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>126</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>126</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>126</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>126</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>126</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>126</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>126</v>
       </c>
@@ -8033,7 +8033,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>126</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>126</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>126</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>126</v>
       </c>
@@ -8134,7 +8134,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>126</v>
       </c>
@@ -8157,7 +8157,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>126</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>126</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>126</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>126</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>126</v>
       </c>
@@ -8281,7 +8281,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>126</v>
       </c>
@@ -8307,7 +8307,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>126</v>
       </c>
@@ -8333,7 +8333,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>126</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>126</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>126</v>
       </c>
@@ -8408,7 +8408,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>126</v>
       </c>
@@ -8431,7 +8431,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>126</v>
       </c>
@@ -8454,7 +8454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>126</v>
       </c>
@@ -8480,7 +8480,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>126</v>
       </c>
@@ -8503,7 +8503,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>126</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>126</v>
       </c>
@@ -8552,7 +8552,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>126</v>
       </c>
@@ -8575,7 +8575,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>126</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>126</v>
       </c>
@@ -8624,7 +8624,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>126</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>126</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>126</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>126</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>126</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>126</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>126</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>126</v>
       </c>
@@ -8823,7 +8823,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>126</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>126</v>
       </c>
@@ -8872,7 +8872,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>126</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>126</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>126</v>
       </c>
@@ -8944,7 +8944,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>126</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>126</v>
       </c>
@@ -8996,7 +8996,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>126</v>
       </c>
@@ -9022,7 +9022,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>126</v>
       </c>
@@ -9048,7 +9048,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>126</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>126</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>126</v>
       </c>
@@ -9126,7 +9126,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>126</v>
       </c>
@@ -9152,7 +9152,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>126</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>126</v>
       </c>
@@ -9204,7 +9204,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>126</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>126</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>126</v>
       </c>
@@ -9279,7 +9279,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>126</v>
       </c>
@@ -9302,7 +9302,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>126</v>
       </c>
@@ -9328,7 +9328,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>126</v>
       </c>
@@ -9351,7 +9351,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>126</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>126</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>126</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>126</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>126</v>
       </c>
@@ -9478,7 +9478,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>126</v>
       </c>
@@ -9504,7 +9504,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>126</v>
       </c>
@@ -9530,7 +9530,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>126</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>126</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>126</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>126</v>
       </c>
@@ -9631,7 +9631,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>126</v>
       </c>
@@ -9657,7 +9657,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>126</v>
       </c>
@@ -9680,7 +9680,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>126</v>
       </c>
@@ -9706,7 +9706,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>126</v>
       </c>
@@ -9729,7 +9729,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>126</v>
       </c>
@@ -9755,7 +9755,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>126</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>126</v>
       </c>
@@ -9807,7 +9807,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>126</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>126</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>126</v>
       </c>
@@ -9882,7 +9882,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>126</v>
       </c>
@@ -9908,7 +9908,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>126</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>126</v>
       </c>
@@ -9954,7 +9954,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>126</v>
       </c>
@@ -9980,7 +9980,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>126</v>
       </c>
@@ -10006,7 +10006,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>126</v>
       </c>
@@ -10032,7 +10032,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>126</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>126</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>126</v>
       </c>
@@ -10107,7 +10107,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>126</v>
       </c>
@@ -10133,7 +10133,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>126</v>
       </c>
@@ -10159,7 +10159,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>126</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>126</v>
       </c>
@@ -10211,7 +10211,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>126</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>126</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>126</v>
       </c>
@@ -10286,7 +10286,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>126</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>126</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>126</v>
       </c>
@@ -10364,7 +10364,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>126</v>
       </c>
@@ -10387,7 +10387,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>126</v>
       </c>
@@ -10413,7 +10413,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>126</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>126</v>
       </c>
@@ -10465,7 +10465,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>126</v>
       </c>
@@ -10491,7 +10491,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>126</v>
       </c>
@@ -10517,7 +10517,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>126</v>
       </c>
@@ -10540,7 +10540,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>126</v>
       </c>
@@ -10563,7 +10563,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>126</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>126</v>
       </c>
@@ -10615,7 +10615,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>126</v>
       </c>
@@ -10641,7 +10641,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>126</v>
       </c>
@@ -10664,7 +10664,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>126</v>
       </c>
@@ -10690,7 +10690,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>126</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>126</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>126</v>
       </c>
@@ -10765,7 +10765,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>126</v>
       </c>
@@ -10791,7 +10791,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>126</v>
       </c>
@@ -10817,7 +10817,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>126</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>126</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>126</v>
       </c>
@@ -10892,7 +10892,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>126</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>126</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>126</v>
       </c>
@@ -10964,7 +10964,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>126</v>
       </c>
@@ -10987,7 +10987,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>126</v>
       </c>
@@ -11010,7 +11010,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>126</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>126</v>
       </c>
@@ -11062,7 +11062,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>126</v>
       </c>
@@ -11088,7 +11088,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>126</v>
       </c>
@@ -11114,7 +11114,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>126</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>126</v>
       </c>
@@ -11163,7 +11163,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>126</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>126</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>126</v>
       </c>
@@ -11235,7 +11235,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>126</v>
       </c>
@@ -11258,7 +11258,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>126</v>
       </c>
@@ -11284,7 +11284,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>126</v>
       </c>
@@ -11307,7 +11307,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>126</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>126</v>
       </c>
@@ -11356,7 +11356,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>126</v>
       </c>
@@ -11382,7 +11382,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>126</v>
       </c>
@@ -11408,7 +11408,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>126</v>
       </c>
@@ -11431,7 +11431,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>126</v>
       </c>
@@ -11454,7 +11454,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>126</v>
       </c>
@@ -11480,7 +11480,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>126</v>
       </c>
@@ -11506,7 +11506,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>126</v>
       </c>
@@ -11529,7 +11529,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>126</v>
       </c>
@@ -11552,7 +11552,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>126</v>
       </c>
@@ -11578,7 +11578,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>126</v>
       </c>
@@ -11601,7 +11601,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>126</v>
       </c>
@@ -11627,7 +11627,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>126</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>126</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>126</v>
       </c>
@@ -11702,7 +11702,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>126</v>
       </c>
@@ -11728,7 +11728,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>126</v>
       </c>
@@ -11754,7 +11754,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>126</v>
       </c>
@@ -11780,7 +11780,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>126</v>
       </c>
@@ -11806,7 +11806,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>126</v>
       </c>
@@ -11832,7 +11832,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>126</v>
       </c>
@@ -11858,7 +11858,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>126</v>
       </c>
@@ -11884,7 +11884,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>126</v>
       </c>
@@ -11910,7 +11910,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>126</v>
       </c>
@@ -11936,7 +11936,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>126</v>
       </c>
@@ -11962,7 +11962,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>126</v>
       </c>
@@ -11988,7 +11988,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>126</v>
       </c>
@@ -12014,7 +12014,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>126</v>
       </c>
@@ -12040,7 +12040,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>126</v>
       </c>
@@ -12063,7 +12063,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>126</v>
       </c>
@@ -12089,7 +12089,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>126</v>
       </c>
@@ -12112,7 +12112,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>126</v>
       </c>
@@ -12138,7 +12138,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>126</v>
       </c>
@@ -12164,7 +12164,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>126</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>126</v>
       </c>
@@ -12213,7 +12213,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>126</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>126</v>
       </c>
@@ -12262,7 +12262,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>126</v>
       </c>
@@ -12288,7 +12288,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>126</v>
       </c>
@@ -12314,7 +12314,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>126</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>126</v>
       </c>
@@ -12363,7 +12363,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>126</v>
       </c>
@@ -12389,7 +12389,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>126</v>
       </c>
@@ -12412,7 +12412,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>126</v>
       </c>
@@ -12438,7 +12438,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>126</v>
       </c>
@@ -12464,7 +12464,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>126</v>
       </c>
@@ -12490,7 +12490,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>126</v>
       </c>
@@ -12516,7 +12516,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>518</v>
       </c>
@@ -12539,7 +12539,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>518</v>
       </c>
@@ -12565,7 +12565,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>518</v>
       </c>
@@ -12591,7 +12591,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>518</v>
       </c>
@@ -12614,7 +12614,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>518</v>
       </c>
@@ -12637,7 +12637,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>518</v>
       </c>
@@ -12663,7 +12663,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>518</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>518</v>
       </c>
@@ -12709,7 +12709,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>518</v>
       </c>
@@ -12732,7 +12732,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>518</v>
       </c>
@@ -12758,7 +12758,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>518</v>
       </c>
@@ -12781,7 +12781,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>518</v>
       </c>
@@ -12804,7 +12804,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="353" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>518</v>
       </c>
@@ -12827,7 +12827,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="354" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>518</v>
       </c>
@@ -12853,7 +12853,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="355" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>518</v>
       </c>
@@ -12879,7 +12879,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="356" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>518</v>
       </c>
@@ -12905,7 +12905,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="357" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>518</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="358" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>518</v>
       </c>
@@ -12957,7 +12957,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="359" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>518</v>
       </c>
@@ -12980,7 +12980,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="360" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>608</v>
       </c>
@@ -13003,7 +13003,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="361" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>608</v>
       </c>
@@ -13026,7 +13026,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="362" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>608</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="363" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>608</v>
       </c>
@@ -13075,7 +13075,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="364" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>608</v>
       </c>
@@ -13101,7 +13101,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="365" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>608</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="366" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>608</v>
       </c>
@@ -13153,7 +13153,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="367" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>608</v>
       </c>
@@ -13179,7 +13179,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="368" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>608</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>608</v>
       </c>
@@ -13225,7 +13225,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>608</v>
       </c>
@@ -13251,7 +13251,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>608</v>
       </c>
@@ -13274,7 +13274,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>608</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>608</v>
       </c>
@@ -13323,7 +13323,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>608</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>608</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>608</v>
       </c>
@@ -13398,7 +13398,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>608</v>
       </c>
@@ -13424,7 +13424,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>608</v>
       </c>
@@ -13450,7 +13450,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>608</v>
       </c>
@@ -13473,7 +13473,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>608</v>
       </c>
@@ -13496,7 +13496,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>608</v>
       </c>
@@ -13522,7 +13522,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>608</v>
       </c>
@@ -13545,7 +13545,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>597</v>
       </c>
@@ -13568,7 +13568,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>597</v>
       </c>
@@ -13594,7 +13594,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>597</v>
       </c>
@@ -13620,7 +13620,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>597</v>
       </c>
@@ -13646,7 +13646,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>597</v>
       </c>
@@ -13672,7 +13672,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>597</v>
       </c>
@@ -13698,7 +13698,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>597</v>
       </c>
@@ -13724,7 +13724,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>597</v>
       </c>
@@ -13750,7 +13750,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>597</v>
       </c>
@@ -13776,7 +13776,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>597</v>
       </c>
@@ -13802,7 +13802,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>597</v>
       </c>
@@ -13828,7 +13828,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>597</v>
       </c>
@@ -13854,7 +13854,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>597</v>
       </c>
@@ -13880,7 +13880,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>597</v>
       </c>
@@ -13906,7 +13906,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>597</v>
       </c>
@@ -13932,7 +13932,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>597</v>
       </c>
@@ -13958,7 +13958,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>597</v>
       </c>
@@ -13984,7 +13984,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>597</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>597</v>
       </c>
@@ -14033,7 +14033,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>597</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>597</v>
       </c>
@@ -14082,7 +14082,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>597</v>
       </c>
@@ -14108,7 +14108,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>597</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>597</v>
       </c>
@@ -14160,7 +14160,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>597</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>597</v>
       </c>
@@ -14212,7 +14212,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>597</v>
       </c>
@@ -14235,7 +14235,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>597</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>597</v>
       </c>
@@ -14287,7 +14287,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>609</v>
       </c>
@@ -14310,7 +14310,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>609</v>
       </c>
@@ -14336,7 +14336,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>609</v>
       </c>
@@ -14363,7 +14363,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G414"/>
+  <autoFilter ref="A1:G414" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>